<commit_message>
updated charts with subtitle
</commit_message>
<xml_diff>
--- a/03-comparing-groups.xlsx
+++ b/03-comparing-groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/kwn5_cdc_gov/Documents/Trainings/2026_EIS-Training/ggplot2-tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{B886F111-FF13-469D-8935-1055F2E75216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5413F9FD-CDC8-40BA-BE4F-FC1F2003FA4B}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{B886F111-FF13-469D-8935-1055F2E75216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAA65039-88F6-4894-8818-B3B1F0A33CF9}"/>
   <bookViews>
-    <workbookView xWindow="38490" yWindow="-4650" windowWidth="29715" windowHeight="18120" activeTab="1" xr2:uid="{D413AA00-99D8-4771-9293-7F2C19E40C6A}"/>
+    <workbookView xWindow="45705" yWindow="-4275" windowWidth="21405" windowHeight="18120" activeTab="1" xr2:uid="{D413AA00-99D8-4771-9293-7F2C19E40C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="1-data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -146,14 +146,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1555,6 +1554,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F77F-41FC-BD52-7E19322B6210}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:numFmt formatCode="General\%" sourceLinked="0"/>
@@ -3016,13 +3020,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>38265</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>64272</xdr:rowOff>
+      <xdr:rowOff>56652</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>382573</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>164</xdr:rowOff>
+      <xdr:rowOff>73269</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3037,8 +3041,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4784200" y="610924"/>
-          <a:ext cx="4634699" cy="664762"/>
+          <a:off x="4771457" y="606171"/>
+          <a:ext cx="4601251" cy="749310"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3097,6 +3101,57 @@
             </a:rPr>
             <a:t>Between 2011 and 2018, e-cigarette use among high school students increased by 19 percentage points.</a:t>
           </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Current use of other tobacco products decreased or did not change.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3143,13 +3198,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>78990</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>114352</xdr:rowOff>
+      <xdr:rowOff>114351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>514159</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>52149</xdr:rowOff>
+      <xdr:colOff>517969</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>43960</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3164,10 +3219,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4812182" y="5426371"/>
-          <a:ext cx="4695922" cy="674300"/>
-          <a:chOff x="4749757" y="6177234"/>
-          <a:chExt cx="4695922" cy="674300"/>
+          <a:off x="4812182" y="5426370"/>
+          <a:ext cx="4692112" cy="847380"/>
+          <a:chOff x="4749757" y="6177233"/>
+          <a:chExt cx="4695922" cy="845475"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -3183,8 +3238,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4749757" y="6177234"/>
-            <a:ext cx="4695922" cy="674300"/>
+            <a:off x="4749757" y="6177233"/>
+            <a:ext cx="4695922" cy="845475"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3243,6 +3298,57 @@
               </a:rPr>
               <a:t>Between 2011        and 2018       ,  e-cigarette use among high school students increased by 19 percentage points.</a:t>
             </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Current use of other tobacco products decreased or did not change.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -3768,7 +3874,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{744E4AEC-917D-40F5-817E-5DCEF51A0701}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{744E4AEC-917D-40F5-817E-5DCEF51A0701}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -4346,8 +4452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B95703E-5E08-45EA-A3AC-DB7F95DDC572}">
   <dimension ref="A3:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4381,10 +4487,10 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>24.2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>27.1</v>
       </c>
     </row>
@@ -4392,10 +4498,10 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>15.8</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>8.1</v>
       </c>
     </row>
@@ -4403,10 +4509,10 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>11.6</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>7.6</v>
       </c>
     </row>
@@ -4414,10 +4520,10 @@
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>1.5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>20.8</v>
       </c>
     </row>
@@ -4425,10 +4531,10 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4436,10 +4542,10 @@
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -4447,10 +4553,10 @@
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>7.9</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>5.9</v>
       </c>
     </row>
@@ -4458,10 +4564,10 @@
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>69.100000000000009</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>74.7</v>
       </c>
     </row>
@@ -4478,10 +4584,10 @@
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -4489,10 +4595,10 @@
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4500,10 +4606,10 @@
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <v>7.9</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>5.9</v>
       </c>
     </row>
@@ -4511,10 +4617,10 @@
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <v>11.6</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>7.6</v>
       </c>
     </row>
@@ -4522,10 +4628,10 @@
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22">
         <v>15.8</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>8.1</v>
       </c>
     </row>
@@ -4533,10 +4639,10 @@
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23">
         <v>1.5</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>20.8</v>
       </c>
     </row>
@@ -4544,10 +4650,10 @@
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24">
         <v>24.2</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24">
         <v>27.1</v>
       </c>
     </row>
@@ -4559,10 +4665,10 @@
       <c r="C31" s="2">
         <v>2018</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4570,10 +4676,10 @@
       <c r="A32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32">
         <v>4</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32">
         <v>1.1000000000000001</v>
       </c>
       <c r="D32">
@@ -4587,10 +4693,10 @@
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33">
         <v>4.0999999999999996</v>
       </c>
       <c r="D33">
@@ -4604,10 +4710,10 @@
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34">
         <v>7.9</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34">
         <v>5.9</v>
       </c>
       <c r="D34">
@@ -4621,10 +4727,10 @@
       <c r="A35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35">
         <v>11.6</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35">
         <v>7.6</v>
       </c>
       <c r="D35">
@@ -4638,10 +4744,10 @@
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36">
         <v>15.8</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36">
         <v>8.1</v>
       </c>
       <c r="D36">
@@ -4655,10 +4761,10 @@
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37">
         <v>1.5</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37">
         <v>20.8</v>
       </c>
       <c r="D37">
@@ -4672,10 +4778,10 @@
       <c r="A38" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38">
         <v>24.2</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38">
         <v>27.1</v>
       </c>
       <c r="D38">

</xml_diff>